<commit_message>
add memmove, memchr and memcmp
</commit_message>
<xml_diff>
--- a/Project1.xlsx
+++ b/Project1.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="54">
   <si>
     <t>Functions - Part 1</t>
   </si>
@@ -32,9 +32,6 @@
   </si>
   <si>
     <t>Marcelo</t>
-  </si>
-  <si>
-    <t>No</t>
   </si>
   <si>
     <t>bzero</t>
@@ -282,10 +279,10 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -294,28 +291,28 @@
     <xf numFmtId="49" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="6" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="6" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="7" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="7" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="7" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -474,13 +471,7 @@
           <a:effectLst/>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
+          <a:effectLst/>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
@@ -579,10 +570,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Cambria"/>
-            <a:ea typeface="Cambria"/>
-            <a:cs typeface="Cambria"/>
-            <a:sym typeface="Cambria"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -837,13 +828,7 @@
           <a:prstDash val="solid"/>
           <a:round/>
         </a:ln>
-        <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
-            <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
+        <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
       <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
@@ -1156,10 +1141,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Cambria"/>
-            <a:ea typeface="Cambria"/>
-            <a:cs typeface="Cambria"/>
-            <a:sym typeface="Cambria"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1424,7 +1409,7 @@
     <col min="3" max="3" width="28.1719" style="1" customWidth="1"/>
     <col min="4" max="4" width="29.1719" style="1" customWidth="1"/>
     <col min="5" max="5" width="22" style="1" customWidth="1"/>
-    <col min="6" max="6" width="37.5078" style="1" customWidth="1"/>
+    <col min="6" max="6" width="37.5" style="1" customWidth="1"/>
     <col min="7" max="256" width="14.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1454,82 +1439,86 @@
       <c r="C2" t="s" s="10">
         <v>6</v>
       </c>
-      <c r="D2" t="s" s="10">
-        <v>7</v>
-      </c>
+      <c r="D2" s="10"/>
       <c r="E2" s="9"/>
       <c r="F2" s="7"/>
     </row>
     <row r="3" ht="17" customHeight="1">
       <c r="A3" t="s" s="8">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="9"/>
       <c r="C3" t="s" s="10">
         <v>6</v>
       </c>
-      <c r="D3" s="9"/>
+      <c r="D3" s="10"/>
       <c r="E3" s="9"/>
       <c r="F3" s="7"/>
     </row>
     <row r="4" ht="17" customHeight="1">
       <c r="A4" t="s" s="8">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" s="9"/>
       <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
+      <c r="D4" s="10"/>
       <c r="E4" s="9"/>
       <c r="F4" s="7"/>
     </row>
     <row r="5" ht="17" customHeight="1">
       <c r="A5" t="s" s="8">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" s="9"/>
       <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
+      <c r="D5" s="10"/>
       <c r="E5" s="9"/>
       <c r="F5" s="7"/>
     </row>
     <row r="6" ht="17" customHeight="1">
       <c r="A6" t="s" s="8">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
+      <c r="C6" t="s" s="10">
+        <v>6</v>
+      </c>
+      <c r="D6" s="10"/>
       <c r="E6" s="9"/>
       <c r="F6" s="7"/>
     </row>
     <row r="7" ht="17" customHeight="1">
       <c r="A7" t="s" s="8">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
+      <c r="C7" t="s" s="10">
+        <v>6</v>
+      </c>
+      <c r="D7" s="10"/>
       <c r="E7" s="9"/>
       <c r="F7" s="7"/>
     </row>
     <row r="8" ht="17" customHeight="1">
       <c r="A8" t="s" s="8">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
+      <c r="C8" t="s" s="10">
+        <v>6</v>
+      </c>
+      <c r="D8" s="10"/>
       <c r="E8" s="9"/>
       <c r="F8" s="7"/>
     </row>
     <row r="9" ht="17" customHeight="1">
       <c r="A9" t="s" s="8">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
       <c r="D9" t="s" s="11">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E9" s="12">
         <v>2</v>
@@ -1538,12 +1527,12 @@
     </row>
     <row r="10" ht="17" customHeight="1">
       <c r="A10" t="s" s="8">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
       <c r="D10" t="s" s="11">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E10" s="12">
         <v>7</v>
@@ -1552,12 +1541,12 @@
     </row>
     <row r="11" ht="17" customHeight="1">
       <c r="A11" t="s" s="8">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
       <c r="D11" t="s" s="11">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E11" s="12">
         <v>4</v>
@@ -1566,12 +1555,12 @@
     </row>
     <row r="12" ht="17" customHeight="1">
       <c r="A12" t="s" s="8">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
       <c r="D12" t="s" s="11">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E12" s="12">
         <v>4</v>
@@ -1580,12 +1569,12 @@
     </row>
     <row r="13" ht="17" customHeight="1">
       <c r="A13" t="s" s="8">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
       <c r="D13" t="s" s="11">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E13" s="12">
         <v>5</v>
@@ -1594,12 +1583,12 @@
     </row>
     <row r="14" ht="17" customHeight="1">
       <c r="A14" t="s" s="8">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
       <c r="D14" t="s" s="11">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E14" s="12">
         <v>5</v>
@@ -1608,12 +1597,12 @@
     </row>
     <row r="15" ht="17" customHeight="1">
       <c r="A15" t="s" s="8">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
       <c r="D15" t="s" s="11">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E15" s="12">
         <v>5</v>
@@ -1622,7 +1611,7 @@
     </row>
     <row r="16" ht="17" customHeight="1">
       <c r="A16" t="s" s="8">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B16" s="9"/>
       <c r="C16" s="9"/>
@@ -1632,7 +1621,7 @@
     </row>
     <row r="17" ht="17" customHeight="1">
       <c r="A17" t="s" s="8">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B17" s="9"/>
       <c r="C17" s="9"/>
@@ -1642,12 +1631,12 @@
     </row>
     <row r="18" ht="17" customHeight="1">
       <c r="A18" t="s" s="8">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B18" s="9"/>
       <c r="C18" s="9"/>
       <c r="D18" t="s" s="11">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E18" s="12">
         <v>4</v>
@@ -1656,7 +1645,7 @@
     </row>
     <row r="19" ht="17" customHeight="1">
       <c r="A19" t="s" s="8">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B19" s="9"/>
       <c r="C19" s="9"/>
@@ -1666,12 +1655,12 @@
     </row>
     <row r="20" ht="17" customHeight="1">
       <c r="A20" t="s" s="8">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
       <c r="D20" t="s" s="11">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E20" s="12">
         <v>4</v>
@@ -1680,12 +1669,12 @@
     </row>
     <row r="21" ht="17" customHeight="1">
       <c r="A21" t="s" s="8">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B21" s="9"/>
       <c r="C21" s="9"/>
       <c r="D21" t="s" s="11">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E21" s="12">
         <v>4</v>
@@ -1694,12 +1683,12 @@
     </row>
     <row r="22" ht="17" customHeight="1">
       <c r="A22" t="s" s="8">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
       <c r="D22" t="s" s="11">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E22" s="12">
         <v>2</v>
@@ -1708,12 +1697,12 @@
     </row>
     <row r="23" ht="17" customHeight="1">
       <c r="A23" t="s" s="8">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
       <c r="D23" t="s" s="11">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E23" s="12">
         <v>5</v>
@@ -1722,28 +1711,28 @@
     </row>
     <row r="24" ht="17" customHeight="1">
       <c r="A24" t="s" s="8">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
       <c r="D24" t="s" s="11">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E24" s="12">
         <v>5</v>
       </c>
       <c r="F24" t="s" s="14">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" ht="17" customHeight="1">
       <c r="A25" t="s" s="8">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B25" s="9"/>
       <c r="C25" s="9"/>
       <c r="D25" t="s" s="11">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E25" s="12">
         <v>5</v>
@@ -1752,28 +1741,28 @@
     </row>
     <row r="26" ht="17" customHeight="1">
       <c r="A26" t="s" s="11">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B26" s="9"/>
       <c r="C26" s="9"/>
       <c r="D26" t="s" s="11">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E26" s="12">
         <v>5</v>
       </c>
       <c r="F26" t="s" s="14">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" ht="17" customHeight="1">
       <c r="A27" t="s" s="8">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
       <c r="D27" t="s" s="11">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E27" s="12">
         <v>5</v>
@@ -1782,12 +1771,12 @@
     </row>
     <row r="28" ht="17" customHeight="1">
       <c r="A28" t="s" s="11">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B28" s="9"/>
       <c r="C28" s="9"/>
       <c r="D28" t="s" s="11">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E28" s="12">
         <v>4</v>
@@ -1796,12 +1785,12 @@
     </row>
     <row r="29" ht="17" customHeight="1">
       <c r="A29" t="s" s="8">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B29" s="9"/>
       <c r="C29" s="9"/>
       <c r="D29" t="s" s="11">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E29" s="12">
         <v>4</v>
@@ -1810,12 +1799,12 @@
     </row>
     <row r="30" ht="17" customHeight="1">
       <c r="A30" t="s" s="8">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B30" s="9"/>
       <c r="C30" s="9"/>
       <c r="D30" t="s" s="11">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E30" s="12">
         <v>2</v>
@@ -1824,7 +1813,7 @@
     </row>
     <row r="31" ht="24" customHeight="1">
       <c r="A31" t="s" s="3">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B31" s="9"/>
       <c r="C31" s="9"/>
@@ -1834,7 +1823,7 @@
     </row>
     <row r="32" ht="17" customHeight="1">
       <c r="A32" t="s" s="8">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B32" s="9"/>
       <c r="C32" s="9"/>
@@ -1844,7 +1833,7 @@
     </row>
     <row r="33" ht="17" customHeight="1">
       <c r="A33" t="s" s="8">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B33" s="9"/>
       <c r="C33" s="9"/>
@@ -1854,7 +1843,7 @@
     </row>
     <row r="34" ht="17" customHeight="1">
       <c r="A34" t="s" s="8">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B34" s="9"/>
       <c r="C34" s="9"/>
@@ -1864,7 +1853,7 @@
     </row>
     <row r="35" ht="17" customHeight="1">
       <c r="A35" t="s" s="8">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B35" s="9"/>
       <c r="C35" s="9"/>
@@ -1874,7 +1863,7 @@
     </row>
     <row r="36" ht="17" customHeight="1">
       <c r="A36" t="s" s="8">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B36" s="9"/>
       <c r="C36" s="9"/>
@@ -1884,7 +1873,7 @@
     </row>
     <row r="37" ht="17" customHeight="1">
       <c r="A37" t="s" s="8">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B37" s="9"/>
       <c r="C37" s="9"/>
@@ -1894,7 +1883,7 @@
     </row>
     <row r="38" ht="17" customHeight="1">
       <c r="A38" t="s" s="8">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B38" s="9"/>
       <c r="C38" s="9"/>
@@ -1904,7 +1893,7 @@
     </row>
     <row r="39" ht="17" customHeight="1">
       <c r="A39" t="s" s="8">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B39" s="9"/>
       <c r="C39" s="9"/>
@@ -1914,7 +1903,7 @@
     </row>
     <row r="40" ht="17" customHeight="1">
       <c r="A40" t="s" s="8">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B40" s="9"/>
       <c r="C40" s="9"/>
@@ -1924,7 +1913,7 @@
     </row>
     <row r="41" ht="17" customHeight="1">
       <c r="A41" t="s" s="8">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B41" s="9"/>
       <c r="C41" s="9"/>
@@ -1934,7 +1923,7 @@
     </row>
     <row r="42" ht="17" customHeight="1">
       <c r="A42" t="s" s="8">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B42" s="9"/>
       <c r="C42" s="9"/>
@@ -1944,7 +1933,7 @@
     </row>
     <row r="43" ht="17" customHeight="1">
       <c r="A43" t="s" s="8">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B43" s="9"/>
       <c r="C43" s="9"/>
@@ -1954,7 +1943,7 @@
     </row>
     <row r="44" ht="17" customHeight="1">
       <c r="A44" t="s" s="8">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B44" s="9"/>
       <c r="C44" s="9"/>
@@ -1964,7 +1953,7 @@
     </row>
     <row r="45" ht="17" customHeight="1">
       <c r="A45" t="s" s="8">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B45" s="9"/>
       <c r="C45" s="9"/>
@@ -1974,7 +1963,7 @@
     </row>
     <row r="46" ht="17" customHeight="1">
       <c r="A46" t="s" s="8">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B46" s="9"/>
       <c r="C46" s="9"/>

</xml_diff>

<commit_message>
updating the file with the functions
</commit_message>
<xml_diff>
--- a/Project1.xlsx
+++ b/Project1.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="57">
   <si>
     <t>Functions - Part 1</t>
   </si>
@@ -638,8 +638,12 @@
       <c r="A26" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
+      <c r="B26" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="D26" s="9" t="s">
         <v>6</v>
       </c>
@@ -791,8 +795,12 @@
       <c r="A38" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B38" s="8"/>
-      <c r="C38" s="8"/>
+      <c r="B38" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>10</v>
+      </c>
       <c r="D38" s="8"/>
       <c r="E38" s="8"/>
     </row>
@@ -852,7 +860,9 @@
       <c r="A43" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B43" s="8"/>
+      <c r="B43" s="7" t="s">
+        <v>6</v>
+      </c>
       <c r="C43" s="7" t="s">
         <v>10</v>
       </c>
@@ -871,11 +881,13 @@
       <c r="E44" s="8"/>
     </row>
     <row r="45">
-      <c r="A45" s="6" t="s">
+      <c r="A45" s="9" t="s">
         <v>55</v>
       </c>
       <c r="B45" s="8"/>
-      <c r="C45" s="7"/>
+      <c r="C45" s="7" t="s">
+        <v>41</v>
+      </c>
       <c r="D45" s="8"/>
       <c r="E45" s="8"/>
     </row>
@@ -887,7 +899,7 @@
         <v>6</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D46" s="8"/>
       <c r="E46" s="8"/>

</xml_diff>